<commit_message>
Cos nie tak z kodowaniem EC
</commit_message>
<xml_diff>
--- a/inst/kodowanieEC.xlsx
+++ b/inst/kodowanieEC.xlsx
@@ -2875,7 +2875,7 @@
   <dimension ref="B1:L125"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A102" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B111" sqref="B111"/>
+      <selection activeCell="B110" sqref="B110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6979,8 +6979,8 @@
     </row>
     <row r="110" spans="2:12">
       <c r="B110" s="2" t="str">
-        <f>"0746"</f>
-        <v>0746</v>
+        <f t="shared" si="10"/>
+        <v>0801</v>
       </c>
       <c r="C110" s="6" t="e">
         <f>#N/A</f>

</xml_diff>